<commit_message>
better handling of spreadsheet values that should be lists
</commit_message>
<xml_diff>
--- a/example-input/E-MTAB-5061-small.xlsx
+++ b/example-input/E-MTAB-5061-small.xlsx
@@ -838,7 +838,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -944,7 +944,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C18" sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1015,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C16" sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1054,7 +1054,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1449,7 +1449,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1518,12 +1518,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="27.83203125" customWidth="1"/>
     <col min="3" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" customWidth="1"/>
@@ -1535,6 +1536,8 @@
     <col min="13" max="13" width="20" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
     <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="16" max="16" width="24.83203125" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -1827,7 +1830,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>